<commit_message>
I was dumb and didnt share this
</commit_message>
<xml_diff>
--- a/api_call/cases.xlsx
+++ b/api_call/cases.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -413,14 +426,84 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>objectIdFieldName</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>globalIdFieldName</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fields</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>exceededTransferLimit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>features</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>uniqueIdField.name</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>uniqueIdField.isSystemMaintained</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ObjectId</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[{'name': 'row_id', 'type': 'esriFieldTypeInteger', 'alias': 'Row ID', 'sqlType': 'sqlTypeInteger', 'domain': None, 'defaultValue': None}, {'name': 'date_reported', 'type': 'esriFieldTypeDate', 'alias': 'Date Reported', 'sqlType': 'sqlTypeTimestamp2', 'length': 8, 'domain': None, 'defaultValue': None}, {'name': 'age_group', 'type': 'esriFieldTypeString', 'alias': 'Age Group', 'sqlType': 'sqlTypeNVarchar', 'length': 2147483647, 'domain': None, 'defaultValue': None}, {'name': 'gender', 'type': 'esriFieldTypeString', 'alias': 'Gender', 'sqlType': 'sqlTypeNVarchar', 'length': 2147483647, 'domain': None, 'defaultValue': None}, {'name': 'province', 'type': 'esriFieldTypeString', 'alias': 'Province Name', 'sqlType': 'sqlTypeNVarchar', 'length': 2147483647, 'domain': None, 'defaultValue': None}, {'name': 'case_status', 'type': 'esriFieldTypeString', 'alias': 'Case Status', 'sqlType': 'sqlTypeNVarchar', 'length': 2147483647, 'domain': None, 'defaultValue': None}, {'name': 'health_region', 'type': 'esriFieldTypeString', 'alias': 'Health Region', 'sqlType': 'sqlTypeNVarchar', 'length': 2147483647, 'domain': None, 'defaultValue': None}]</t>
+        </is>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[{'attributes': {'row_id': 500, 'date_reported': 1600430400000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 1000, 'date_reported': 1603108800000, 'age_group': '70-79', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Windsor-Essex County Health Unit'}}, {'attributes': {'row_id': 501, 'date_reported': 1602331200000, 'age_group': '50-59', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 502, 'date_reported': 1595592000000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 503, 'date_reported': 1599048000000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 504, 'date_reported': 1601121600000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 505, 'date_reported': 1599912000000, 'age_group': '50-59', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 506, 'date_reported': 1603368000000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 507, 'date_reported': 1601812800000, 'age_group': '60-69', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 508, 'date_reported': 1601985600000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 509, 'date_reported': 1600948800000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 510, 'date_reported': 1600776000000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 511, 'date_reported': 1601467200000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 512, 'date_reported': 1600084800000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 513, 'date_reported': 1602331200000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 514, 'date_reported': 1600689600000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Eastern Ontario Health Unit'}}, {'attributes': {'row_id': 515, 'date_reported': 1599652800000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 516, 'date_reported': 1603368000000, 'age_group': '70-79', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 517, 'date_reported': 1601035200000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 518, 'date_reported': 1603972800000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Niagara Region Public Health Department'}}, {'attributes': {'row_id': 519, 'date_reported': 1601726400000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Simcoe Muskoka District Health Unit'}}, {'attributes': {'row_id': 520, 'date_reported': 1603540800000, 'age_group': '80+', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 521, 'date_reported': 1601121600000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 522, 'date_reported': 1600084800000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 523, 'date_reported': 1602417600000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 524, 'date_reported': 1595073600000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 525, 'date_reported': 1603454400000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 526, 'date_reported': 1603540800000, 'age_group': '60-69', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 527, 'date_reported': 1602158400000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 528, 'date_reported': 1599912000000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Haliburton, Kawartha, Pine Ridge District Health Unit'}}, {'attributes': {'row_id': 529, 'date_reported': 1595764800000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 530, 'date_reported': 1603022400000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 531, 'date_reported': 1604145600000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 532, 'date_reported': 1599825600000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 533, 'date_reported': 1602676800000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 534, 'date_reported': 1598097600000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 535, 'date_reported': 1603454400000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 536, 'date_reported': 1604404800000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Hamilton Public Health Services'}}, {'attributes': {'row_id': 537, 'date_reported': 1603281600000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 538, 'date_reported': 1603368000000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 0, 'date_reported': 1604059200000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Southwestern Public Health'}}, {'attributes': {'row_id': 2000, 'date_reported': 1599652800000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 1500, 'date_reported': 1601294400000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 539, 'date_reported': 1599825600000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 540, 'date_reported': 1600516800000, 'age_group': '70-79', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 541, 'date_reported': 1603713600000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 542, 'date_reported': 1602676800000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Wellington-Dufferin-Guelph Public Health'}}, {'attributes': {'row_id': 543, 'date_reported': 1603713600000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Hamilton Public Health Services'}}, {'attributes': {'row_id': 544, 'date_reported': 1601812800000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 545, 'date_reported': 1599912000000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Hamilton Public Health Services'}}, {'attributes': {'row_id': 546, 'date_reported': 1602849600000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Brant County Health Unit'}}, {'attributes': {'row_id': 547, 'date_reported': 1604404800000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Wellington-Dufferin-Guelph Public Health'}}, {'attributes': {'row_id': 548, 'date_reported': 1603713600000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 549, 'date_reported': 1602244800000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 550, 'date_reported': 1602504000000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 551, 'date_reported': 1598270400000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Windsor-Essex County Health Unit'}}, {'attributes': {'row_id': 552, 'date_reported': 1603454400000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 553, 'date_reported': 1600689600000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 554, 'date_reported': 1599393600000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 555, 'date_reported': 1604232000000, 'age_group': '20-29', 'gender': 'Not Reported', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 556, 'date_reported': 1600430400000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 557, 'date_reported': 1601035200000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 558, 'date_reported': 1602072000000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 559, 'date_reported': 1601380800000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 560, 'date_reported': 1603195200000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Windsor-Essex County Health Unit'}}, {'attributes': {'row_id': 561, 'date_reported': 1601467200000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 562, 'date_reported': 1603713600000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 563, 'date_reported': 1601553600000, 'age_group': '60-69', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 564, 'date_reported': 1603022400000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 565, 'date_reported': 1601035200000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 566, 'date_reported': 1600171200000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Windsor-Essex County Health Unit'}}, {'attributes': {'row_id': 567, 'date_reported': 1601985600000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 568, 'date_reported': 1604145600000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 569, 'date_reported': 1601294400000, 'age_group': '70-79', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 570, 'date_reported': 1601035200000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 571, 'date_reported': 1604145600000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 572, 'date_reported': 1603540800000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 573, 'date_reported': 1603972800000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 574, 'date_reported': 1599739200000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 575, 'date_reported': 1603540800000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 576, 'date_reported': 1599652800000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 577, 'date_reported': 1600862400000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Sudbury &amp; District Health Unit'}}, {'attributes': {'row_id': 578, 'date_reported': 1604404800000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Kingston, Frontenac and Lennox &amp; Addington Public Health'}}, {'attributes': {'row_id': 579, 'date_reported': 1603886400000, 'age_group': '60-69', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Haldimand-Norfolk Health Unit'}}, {'attributes': {'row_id': 580, 'date_reported': 1604404800000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 581, 'date_reported': 1603368000000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 582, 'date_reported': 1601380800000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 583, 'date_reported': 1596974400000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 584, 'date_reported': 1602504000000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 585, 'date_reported': 1603368000000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 586, 'date_reported': 1601640000000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 587, 'date_reported': 1600516800000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 588, 'date_reported': 1603195200000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 589, 'date_reported': 1599220800000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 590, 'date_reported': 1601985600000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 591, 'date_reported': 1604145600000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Simcoe Muskoka District Health Unit'}}, {'attributes': {'row_id': 592, 'date_reported': 1603022400000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Durham Region Health Department'}}, {'attributes': {'row_id': 593, 'date_reported': 1597320000000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 594, 'date_reported': 1595332800000, 'age_group': '50-59', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 595, 'date_reported': 1601899200000, 'age_group': '70-79', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 596, 'date_reported': 1601035200000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 597, 'date_reported': 1603368000000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 598, 'date_reported': 1603627200000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Durham Region Health Department'}}, {'attributes': {'row_id': 599, 'date_reported': 1600430400000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 600, 'date_reported': 1599825600000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 601, 'date_reported': 1601640000000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Niagara Region Public Health Department'}}, {'attributes': {'row_id': 602, 'date_reported': 1601985600000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Durham Region Health Department'}}, {'attributes': {'row_id': 603, 'date_reported': 1600948800000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 604, 'date_reported': 1601294400000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 605, 'date_reported': 1601899200000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Renfrew County and District Health Unit'}}, {'attributes': {'row_id': 606, 'date_reported': 1604577600000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 607, 'date_reported': 1603108800000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 608, 'date_reported': 1599825600000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 609, 'date_reported': 1603108800000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Brant County Health Unit'}}, {'attributes': {'row_id': 610, 'date_reported': 1603886400000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 611, 'date_reported': 1599480000000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 612, 'date_reported': 1601380800000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 1001, 'date_reported': 1601294400000, 'age_group': '60-69', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Eastern Ontario Health Unit'}}, {'attributes': {'row_id': 613, 'date_reported': 1603800000000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 614, 'date_reported': 1602590400000, 'age_group': '&lt;20', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 615, 'date_reported': 1602763200000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 616, 'date_reported': 1603713600000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 617, 'date_reported': 1604145600000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 618, 'date_reported': 1604318400000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 619, 'date_reported': 1604318400000, 'age_group': '70-79', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 620, 'date_reported': 1600516800000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 621, 'date_reported': 1599825600000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 622, 'date_reported': 1602158400000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 623, 'date_reported': 1602158400000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Simcoe Muskoka District Health Unit'}}, {'attributes': {'row_id': 624, 'date_reported': 1602590400000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Durham Region Health Department'}}, {'attributes': {'row_id': 625, 'date_reported': 1602849600000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 626, 'date_reported': 1604404800000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 627, 'date_reported': 1604059200000, 'age_group': '40-49', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 628, 'date_reported': 1595246400000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 629, 'date_reported': 1602331200000, 'age_group': '20-29', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 630, 'date_reported': 1603627200000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 631, 'date_reported': 1603886400000, 'age_group': '50-59', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Durham Region Health Department'}}, {'attributes': {'row_id': 632, 'date_reported': 1603195200000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 633, 'date_reported': 1601899200000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 634, 'date_reported': 1601985600000, 'age_group': '50-59', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 635, 'date_reported': 1604232000000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Niagara Region Public Health Department'}}, {'attributes': {'row_id': 636, 'date_reported': 1600776000000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Leeds, Grenville and Lanark District Health Unit'}}, {'attributes': {'row_id': 637, 'date_reported': 1604404800000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 638, 'date_reported': 1601467200000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 639, 'date_reported': 1603281600000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Hamilton Public Health Services'}}, {'attributes': {'row_id': 640, 'date_reported': 1600776000000, 'age_group': '30-39', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 641, 'date_reported': 1603627200000, 'age_group': '70-79', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Brant County Health Unit'}}, {'attributes': {'row_id': 642, 'date_reported': 1601899200000, 'age_group': '60-69', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 643, 'date_reported': 1601726400000, 'age_group': '70-79', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 644, 'date_reported': 1602158400000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 645, 'date_reported': 1604232000000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 646, 'date_reported': 1600171200000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 647, 'date_reported': 1604577600000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Active', 'health_region': 'Halton Region Health Department'}}, {'attributes': {'row_id': 648, 'date_reported': 1600344000000, 'age_group': '&lt;20', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 649, 'date_reported': 1601553600000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Peel Public Health'}}, {'attributes': {'row_id': 650, 'date_reported': 1600257600000, 'age_group': '50-59', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 651, 'date_reported': 1602590400000, 'age_group': '40-49', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'York Region Public Health Services'}}, {'attributes': {'row_id': 652, 'date_reported': 1602590400000, 'age_group': '60-69', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 653, 'date_reported': 1601899200000, 'age_group': '30-39', 'gender': 'Female', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Haldimand-Norfolk Health Unit'}}, {'attributes': {'row_id': 654, 'date_reported': 1600776000000, 'age_group': '20-29', 'gender': 'Male', 'province': 'Ontario', 'case_status': 'Recovered', 'health_region': 'Region of Waterloo, Public Health'}}, {'attributes': {'row_id': 655, 'date_reported':</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ObjectId</t>
+        </is>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>